<commit_message>
pcof other info and cash data fix
</commit_message>
<xml_diff>
--- a/Frontend/src/assets/template File/PCOF - Other Info.xlsx
+++ b/Frontend/src/assets/template File/PCOF - Other Info.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28814"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Disha\Downloads\Borrowing Base FIGMA working FIles\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA4D9A55-897E-427A-8A1C-EAE66A0ED622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="8" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" firstSheet="4" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Availability Borrower" sheetId="19" r:id="rId1"/>
@@ -22,9 +16,9 @@
     <sheet name="Concentration Limits" sheetId="16" r:id="rId7"/>
     <sheet name="MV and BV 4.30" sheetId="9" state="hidden" r:id="rId8"/>
     <sheet name="Other Metrics" sheetId="18" r:id="rId9"/>
+    <sheet name="Obligors' Net Capital" sheetId="23" r:id="rId10"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId10"/>
     <externalReference r:id="rId11"/>
     <externalReference r:id="rId12"/>
     <externalReference r:id="rId13"/>
@@ -577,7 +571,8 @@
     <definedName name="lookup_errorcodes">[11]SelectLists!$O$4:$P$13</definedName>
     <definedName name="LookupArrayAfter">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="124519"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -597,79 +592,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="ing me"/>
-            <charset val="1"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>======
-ID#AAAAyLBFivA
-Troxel, Richard    (2023-05-30 21:05:02)
-Placeholder; to be updated</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0D00-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="ing me"/>
-            <charset val="1"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>======
-ID#AAAAyLBFivE
-Troxel, Richard    (2023-05-30 21:05:02)
-Including Performing DIP</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0D00-000002000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="ing me"/>
-            <charset val="1"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>======
-ID#AAAAyLBFiu8
-Troxel, Richard    (2023-05-30 21:05:02)
-Including Unsecured High Yield</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="151">
   <si>
     <t>A</t>
   </si>
@@ -1096,19 +1020,46 @@
   <si>
     <t>Threshold 2 Advance Rate</t>
   </si>
+  <si>
+    <t>Obligors' Net Capital</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>Equity Paid in Capital</t>
+  </si>
+  <si>
+    <t>Distributions</t>
+  </si>
+  <si>
+    <t>Retained Earnings</t>
+  </si>
+  <si>
+    <t>(a) Partners' Capital</t>
+  </si>
+  <si>
+    <t>(b) Uncalled Capital Commitments (excl. Defaulting Investors)</t>
+  </si>
+  <si>
+    <t>Obligors' Net Capital ((a) + (b))</t>
+  </si>
+  <si>
+    <t>Debt / Equity</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="0.00\x;\(0.00\x\);\-"/>
-    <numFmt numFmtId="165" formatCode="#,##0.0;\(#,##0.0\);\-"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.00\x;\(0.00\x\);\-"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0;\(#,##0.0\);\-"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1141,13 +1092,6 @@
       <color theme="1"/>
       <name val="ing me"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="ing me"/>
-      <charset val="1"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1211,6 +1155,19 @@
       <sz val="8"/>
       <color rgb="FF1E5680"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1478,176 +1435,178 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="8" fillId="5" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="7" fillId="5" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="5" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="10" fillId="5" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="5" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="7" fillId="5" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="5" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="7" fillId="5" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="5" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="7" fillId="5" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="7" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="8" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="7" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="14" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="13" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="14" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="13" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="10" fontId="8" fillId="5" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="7" fillId="5" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="8" fillId="5" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="7" fillId="5" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="8" fillId="5" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="7" fillId="5" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="8" fillId="5" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="7" fillId="5" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="8" fillId="5" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="7" fillId="5" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="8" fillId="5" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="7" fillId="5" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="8" fillId="5" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="7" fillId="5" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="10" fontId="8" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="7" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1668,7 +1627,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Summary Slides All Debt"/>
@@ -1711,7 +1670,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink10.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Borrowing Request"/>
@@ -1744,7 +1703,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink11.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Instructions"/>
@@ -1792,21 +1751,8 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink12.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Inputs"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Borrowing Request"/>
@@ -1837,7 +1783,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Borrowing Base Certificate"/>
@@ -1862,7 +1808,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Floaters"/>
@@ -1881,7 +1827,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Table of Contents"/>
@@ -1972,7 +1918,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Compliance"/>
@@ -2015,7 +1961,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink7.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="All Debt"/>
@@ -2074,7 +2020,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink8.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Year"/>
@@ -2101,7 +2047,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink9.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Cash flow Calculation"/>
@@ -2348,14 +2294,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="47" customWidth="1"/>
     <col min="2" max="2" width="28.25" customWidth="1"/>
@@ -2369,7 +2315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" ht="14.25">
       <c r="A2" s="52" t="s">
         <v>2</v>
       </c>
@@ -2377,7 +2323,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" ht="14.25">
       <c r="A3" s="10" t="s">
         <v>4</v>
       </c>
@@ -2385,7 +2331,7 @@
         <v>45230</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" ht="14.25">
       <c r="A4" s="11" t="s">
         <v>5</v>
       </c>
@@ -2393,7 +2339,7 @@
         <v>44914</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="14.25">
       <c r="A5" s="52" t="s">
         <v>6</v>
       </c>
@@ -2401,7 +2347,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" ht="14.25">
       <c r="A6" s="53" t="s">
         <v>8</v>
       </c>
@@ -2409,7 +2355,7 @@
         <v>60000000</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" ht="14.25">
       <c r="A7" s="54" t="s">
         <v>9</v>
       </c>
@@ -2433,9 +2379,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+  <extLst xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
+    <ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
@@ -2449,21 +2394,104 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="32.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="14.25">
+      <c r="A1" s="74" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="74" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="14.25">
+      <c r="A2" s="75" t="s">
+        <v>144</v>
+      </c>
+      <c r="B2" s="75">
+        <v>22875000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="14.25">
+      <c r="A3" s="75" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" s="75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="14.25">
+      <c r="A4" s="75" t="s">
+        <v>146</v>
+      </c>
+      <c r="B4" s="75">
+        <v>1174447</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14.25">
+      <c r="A5" s="75" t="s">
+        <v>147</v>
+      </c>
+      <c r="B5" s="75">
+        <v>24049447</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="14.25">
+      <c r="A6" s="75" t="s">
+        <v>148</v>
+      </c>
+      <c r="B6" s="75">
+        <v>53375000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="14.25">
+      <c r="A7" s="75" t="s">
+        <v>149</v>
+      </c>
+      <c r="B7" s="75">
+        <v>77424447</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="14.25">
+      <c r="A8" s="75" t="s">
+        <v>150</v>
+      </c>
+      <c r="B8" s="75">
+        <v>2.4948598610000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A64CF9C-2F15-4BC6-991C-6BD263061325}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="3" max="3" width="9.25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" ht="14.25">
       <c r="A1" s="32" t="s">
         <v>11</v>
       </c>
@@ -2480,7 +2508,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" ht="14.25">
       <c r="A2" s="14" t="s">
         <v>9</v>
       </c>
@@ -2530,14 +2558,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEFBC228-6345-4726-B100-E5AECE567F7F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView topLeftCell="A26" workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
@@ -2547,7 +2575,7 @@
     <col min="6" max="6" width="7.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31.15">
+    <row r="1" spans="1:6" ht="33.75">
       <c r="A1" s="37" t="s">
         <v>18</v>
       </c>
@@ -2567,7 +2595,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" ht="14.25">
       <c r="A2" s="38" t="s">
         <v>24</v>
       </c>
@@ -2583,7 +2611,7 @@
         <v>4500000</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" ht="14.25">
       <c r="A3" s="39" t="s">
         <v>26</v>
       </c>
@@ -2599,7 +2627,7 @@
         <v>6000000</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" ht="14.25">
       <c r="A4" s="39" t="s">
         <v>27</v>
       </c>
@@ -2615,7 +2643,7 @@
         <v>1500000</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" ht="14.25">
       <c r="A5" s="39" t="s">
         <v>28</v>
       </c>
@@ -2631,7 +2659,7 @@
         <v>1500000</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" ht="14.25">
       <c r="A6" s="39" t="s">
         <v>29</v>
       </c>
@@ -2647,7 +2675,7 @@
         <v>900000</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" ht="14.25">
       <c r="A7" s="39" t="s">
         <v>30</v>
       </c>
@@ -2663,7 +2691,7 @@
         <v>1200000</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" ht="14.25">
       <c r="A8" s="39" t="s">
         <v>31</v>
       </c>
@@ -2679,7 +2707,7 @@
         <v>1200000</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" ht="14.25">
       <c r="A9" s="39" t="s">
         <v>32</v>
       </c>
@@ -2695,7 +2723,7 @@
         <v>1500000</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" ht="14.25">
       <c r="A10" s="39"/>
       <c r="B10" s="40"/>
       <c r="C10" s="44"/>
@@ -2705,7 +2733,7 @@
       <c r="E10" s="46"/>
       <c r="F10" s="46"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" ht="14.25">
       <c r="A11" s="39"/>
       <c r="B11" s="40"/>
       <c r="C11" s="44"/>
@@ -2715,7 +2743,7 @@
       <c r="E11" s="46"/>
       <c r="F11" s="46"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" ht="14.25">
       <c r="A12" s="39"/>
       <c r="B12" s="40"/>
       <c r="C12" s="44"/>
@@ -2725,7 +2753,7 @@
       <c r="E12" s="46"/>
       <c r="F12" s="46"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" ht="14.25">
       <c r="A13" s="39"/>
       <c r="B13" s="40"/>
       <c r="C13" s="44"/>
@@ -2735,7 +2763,7 @@
       <c r="E13" s="46"/>
       <c r="F13" s="46"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" ht="14.25">
       <c r="A14" s="39"/>
       <c r="B14" s="40"/>
       <c r="C14" s="44"/>
@@ -2745,7 +2773,7 @@
       <c r="E14" s="46"/>
       <c r="F14" s="46"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" ht="14.25">
       <c r="A15" s="39"/>
       <c r="B15" s="40"/>
       <c r="C15" s="44"/>
@@ -2755,7 +2783,7 @@
       <c r="E15" s="46"/>
       <c r="F15" s="46"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" ht="14.25">
       <c r="A16" s="39"/>
       <c r="B16" s="40"/>
       <c r="C16" s="44"/>
@@ -2765,7 +2793,7 @@
       <c r="E16" s="46"/>
       <c r="F16" s="46"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" ht="14.25">
       <c r="A17" s="39"/>
       <c r="B17" s="40"/>
       <c r="C17" s="44"/>
@@ -2775,7 +2803,7 @@
       <c r="E17" s="46"/>
       <c r="F17" s="46"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" ht="14.25">
       <c r="A18" s="39"/>
       <c r="B18" s="40"/>
       <c r="C18" s="44"/>
@@ -2785,7 +2813,7 @@
       <c r="E18" s="46"/>
       <c r="F18" s="46"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" ht="14.25">
       <c r="A19" s="39"/>
       <c r="B19" s="40"/>
       <c r="C19" s="44"/>
@@ -2795,7 +2823,7 @@
       <c r="E19" s="46"/>
       <c r="F19" s="46"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" ht="14.25">
       <c r="A20" s="39"/>
       <c r="B20" s="40"/>
       <c r="C20" s="44"/>
@@ -2805,7 +2833,7 @@
       <c r="E20" s="46"/>
       <c r="F20" s="46"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" ht="14.25">
       <c r="A21" s="39"/>
       <c r="B21" s="40"/>
       <c r="C21" s="44"/>
@@ -2815,7 +2843,7 @@
       <c r="E21" s="46"/>
       <c r="F21" s="46"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" ht="14.25">
       <c r="A22" s="47" t="s">
         <v>33</v>
       </c>
@@ -2831,7 +2859,7 @@
         <v>1500000</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" ht="14.25">
       <c r="A23" s="47" t="s">
         <v>35</v>
       </c>
@@ -2847,7 +2875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" ht="14.25">
       <c r="A24" s="47" t="s">
         <v>36</v>
       </c>
@@ -2863,7 +2891,7 @@
         <v>450000</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" ht="14.25">
       <c r="A25" s="47" t="s">
         <v>37</v>
       </c>
@@ -2879,7 +2907,7 @@
         <v>2400000</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" ht="14.25">
       <c r="A26" s="47" t="s">
         <v>38</v>
       </c>
@@ -2895,7 +2923,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" ht="14.25">
       <c r="A27" s="47" t="s">
         <v>39</v>
       </c>
@@ -2911,7 +2939,7 @@
         <v>75000</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" ht="14.25">
       <c r="A28" s="47"/>
       <c r="B28" s="47"/>
       <c r="C28" s="47"/>
@@ -2923,7 +2951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" ht="14.25">
       <c r="A29" s="47"/>
       <c r="B29" s="47"/>
       <c r="C29" s="47"/>
@@ -2935,7 +2963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" ht="14.25">
       <c r="A30" s="47" t="s">
         <v>40</v>
       </c>
@@ -2949,7 +2977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" ht="14.25">
       <c r="A31" s="47" t="s">
         <v>41</v>
       </c>
@@ -2963,7 +2991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" ht="14.25">
       <c r="A32" s="47" t="s">
         <v>42</v>
       </c>
@@ -2977,7 +3005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" ht="14.25">
       <c r="A33" s="47" t="s">
         <v>43</v>
       </c>
@@ -2991,7 +3019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" ht="14.25">
       <c r="A34" s="47" t="s">
         <v>44</v>
       </c>
@@ -3005,7 +3033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" ht="14.25">
       <c r="A35" s="48"/>
       <c r="B35" s="49"/>
       <c r="C35" s="49"/>
@@ -3021,20 +3049,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="45" customWidth="1"/>
     <col min="2" max="2" width="9" style="60"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="14.25">
       <c r="A1" s="72" t="s">
         <v>46</v>
       </c>
@@ -3050,7 +3078,7 @@
         <v>2.2499999999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" ht="14.25">
       <c r="A3" s="23"/>
       <c r="B3" s="62"/>
     </row>
@@ -3100,20 +3128,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="22.125" customWidth="1"/>
     <col min="2" max="2" width="9.875" style="60" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="14.25">
       <c r="A1" s="6" t="s">
         <v>54</v>
       </c>
@@ -3121,7 +3149,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" ht="14.25">
       <c r="A2" s="27" t="s">
         <v>25</v>
       </c>
@@ -3129,7 +3157,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" ht="14.25">
       <c r="A3" s="28" t="s">
         <v>56</v>
       </c>
@@ -3137,7 +3165,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" ht="14.25">
       <c r="A4" s="29" t="s">
         <v>45</v>
       </c>
@@ -3151,20 +3179,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="14.375" customWidth="1"/>
     <col min="2" max="3" width="9" style="60"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" ht="14.25">
       <c r="A1" s="6" t="s">
         <v>57</v>
       </c>
@@ -3320,25 +3348,24 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
     <col min="3" max="3" width="13.75" style="60" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" ht="14.25">
       <c r="A1" s="6" t="s">
         <v>73</v>
       </c>
@@ -3349,7 +3376,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" ht="14.25">
       <c r="A2" s="29" t="s">
         <v>76</v>
       </c>
@@ -3358,7 +3385,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" ht="14.25">
       <c r="A3" s="29" t="s">
         <v>77</v>
       </c>
@@ -3367,7 +3394,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" ht="14.25">
       <c r="A4" s="29" t="s">
         <v>78</v>
       </c>
@@ -3382,7 +3409,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -32426,20 +32453,20 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9:B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="25.25" customWidth="1"/>
     <col min="2" max="2" width="5.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="14.25">
       <c r="A1" s="4" t="s">
         <v>128</v>
       </c>
@@ -32447,7 +32474,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" ht="14.25">
       <c r="A2" s="14" t="s">
         <v>130</v>
       </c>
@@ -32455,7 +32482,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" ht="14.25">
       <c r="A3" s="14" t="s">
         <v>131</v>
       </c>
@@ -32463,7 +32490,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" ht="14.25">
       <c r="A4" s="14" t="s">
         <v>132</v>
       </c>
@@ -32471,13 +32498,13 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="14.25">
       <c r="A5" s="14" t="s">
         <v>133</v>
       </c>
       <c r="B5" s="8"/>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" ht="14.25">
       <c r="A6" s="11" t="s">
         <v>134</v>
       </c>
@@ -32485,7 +32512,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" ht="14.25">
       <c r="A7" s="11" t="s">
         <v>135</v>
       </c>
@@ -32493,7 +32520,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" ht="14.25">
       <c r="A8" s="11" t="s">
         <v>136</v>
       </c>
@@ -32559,6 +32586,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E2D6C0B0299502459BE057F60D45F7A2" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f50657443db3cca893bf2a77a6b82c8e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ecf2865c-a0c0-4830-9c97-c878b24eefc5" xmlns:ns3="0c3f3349-3fde-44b2-91dd-1461469ae59c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ffe86a2076484ea9f4ac21488ba3d86b" ns2:_="" ns3:_="">
     <xsd:import namespace="ecf2865c-a0c0-4830-9c97-c878b24eefc5"/>
@@ -32799,23 +32835,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCF8A72F-D295-4574-82B8-441B0398744E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCF8A72F-D295-4574-82B8-441B0398744E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0c3f3349-3fde-44b2-91dd-1461469ae59c"/>
+    <ds:schemaRef ds:uri="ecf2865c-a0c0-4830-9c97-c878b24eefc5"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0B1DE2C-B754-4698-8D14-ED482BBE5558}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A217E5FC-6AA4-4D58-87BB-3869865F3C89}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A217E5FC-6AA4-4D58-87BB-3869865F3C89}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0B1DE2C-B754-4698-8D14-ED482BBE5558}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ecf2865c-a0c0-4830-9c97-c878b24eefc5"/>
+    <ds:schemaRef ds:uri="0c3f3349-3fde-44b2-91dd-1461469ae59c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>